<commit_message>
NHD diagnosis and mortality
</commit_message>
<xml_diff>
--- a/Parameters bladder cancer model.xlsx
+++ b/Parameters bladder cancer model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cm1om\Documents\Research\Cancer\Bladder\Bladder_cancer_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD16470-B89C-4C3A-9C1A-0C2F11BA2CEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A0A769-41C1-468F-AA8A-754F1380FE63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{1AD6D928-CCB7-482A-A47C-26785A7D3A52}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="106">
   <si>
     <t>Param number</t>
   </si>
@@ -165,15 +165,6 @@
   </si>
   <si>
     <t>p that at a time of onset (t0) the tumour is low-risk</t>
-  </si>
-  <si>
-    <t>Proportion of patients progressing from low-risk BC to MIBC</t>
-  </si>
-  <si>
-    <t>Probability to die from BC if you have low-risk non-MIBC</t>
-  </si>
-  <si>
-    <t>Among LR patients with the median followup was 61 months (IQR 24–105). Of the patients 17 (2.4%) died of bladder cancer</t>
   </si>
   <si>
     <t xml:space="preserve">Recurrence developed in 199 patients (28.5%, 95%
@@ -187,12 +178,6 @@
     <t>Assumption based on clinical study from Linton et al (2013) http://dx.doi.org/10.1016/j.juro.2012.09.084</t>
   </si>
   <si>
-    <t>Assumptions based on clinical experts input</t>
-  </si>
-  <si>
-    <t>P.LRtoMIBC</t>
-  </si>
-  <si>
     <t>P.Recurrence.LR</t>
   </si>
   <si>
@@ -295,12 +280,6 @@
     <t>Age (for those who are older than 80) coefficient in the equation for Probability to have symptomatic diagnosis with potentially invasive cancer as a function of time since cancer onset</t>
   </si>
   <si>
-    <t xml:space="preserve">Time coefficient (years subce onset) in the equation for Probability to become a symptomatic patient by time with high grade BC  (y= a*b^t+K(age)*[age&gt;80-age]) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">A coefficient (intercept) in the Probability to become a symptomatic patient by time with high grade BC (y= a*b^t+K(age)*[age&gt;80-age]) </t>
-  </si>
-  <si>
     <t>P.sympt.diag_LGBC</t>
   </si>
   <si>
@@ -338,6 +317,45 @@
   </si>
   <si>
     <t>Mean.t.StIII.StIV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A coefficient (intercept) in the Probability to become a symptomatic patient by time with high grade BC (y= a*b^t *(K(age)^[age&gt;80-age]) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time coefficient (years subce onset) in the equation for Probability to become a symptomatic patient by time with high grade BC  (y= a*b^t+(K(age)^[age&gt;80-age]) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RR of all cause mortality for non-smokers compared to the whole population </t>
+  </si>
+  <si>
+    <t>RR.All.Death.no_smoke</t>
+  </si>
+  <si>
+    <t>shape.t.StI.StII</t>
+  </si>
+  <si>
+    <t>shape.t.StII.StIII</t>
+  </si>
+  <si>
+    <t>shape.t.StIII.StIV</t>
+  </si>
+  <si>
+    <t>shape time of BC development from Stage I to Stage II</t>
+  </si>
+  <si>
+    <t>shape time of BC development from Stage II to Stage III</t>
+  </si>
+  <si>
+    <t>shape time of BC development from Stage III to Stage IV</t>
+  </si>
+  <si>
+    <t>Among LR patients with the median followup was 61 months (IQR 24–105). Of the patients 17 (2.4%) died of bladder cancer. Calculated as 0.0048 annually (2.4% during 5 years)</t>
+  </si>
+  <si>
+    <t>Proportion of patients progressing from low-grade BC to HGBC</t>
+  </si>
+  <si>
+    <t>P.LGtoHGBC</t>
   </si>
 </sst>
 </file>
@@ -383,7 +401,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -398,25 +416,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -440,7 +440,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -456,27 +456,21 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -792,10 +786,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8694223C-410D-4023-9128-3FD5F8A481E4}">
-  <dimension ref="A1:X39"/>
+  <dimension ref="A1:X38"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:B19"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -833,14 +827,14 @@
       <c r="F1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="15"/>
-      <c r="I1" s="16" t="s">
+      <c r="H1" s="12"/>
+      <c r="I1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="16"/>
+      <c r="J1" s="13"/>
       <c r="K1" s="2" t="s">
         <v>7</v>
       </c>
@@ -851,362 +845,362 @@
         <v>12</v>
       </c>
       <c r="O1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:24" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="7">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="E2" s="7">
+      <c r="C2" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="5">
         <v>1E-4</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="5">
         <v>1</v>
       </c>
-      <c r="G2" s="7">
+      <c r="G2" s="5">
         <f>((1-E2)/(K2^2)^2 -1/E2)*E2^2</f>
         <v>0.99980000000000002</v>
       </c>
-      <c r="H2" s="7">
+      <c r="H2" s="5">
         <f>G2*(1/E2-1)</f>
         <v>9997.0002000000004</v>
       </c>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7">
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5">
         <v>0.01</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="L2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="M2" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="T2" s="13" t="s">
+      <c r="T2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="U2" s="13" t="s">
+      <c r="U2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="V2" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="W2" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="X2" s="13" t="s">
-        <v>66</v>
+      <c r="V2" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="W2" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="X2" s="9" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="7">
+      <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="5">
         <v>0.192</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="5">
         <v>1</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="5">
         <f>((1-E3)/(K3^2)^2 -1/E3)*E3^2</f>
         <v>4765.5859199999986</v>
       </c>
-      <c r="H3" s="7">
+      <c r="H3" s="5">
         <f>G3*(1/E3-1)</f>
         <v>20055.174079999993</v>
       </c>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7">
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5">
         <v>0.05</v>
       </c>
-      <c r="L3" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="M3" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="T3" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="U3" s="13">
+      <c r="L3" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="T3" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="U3" s="9">
         <v>0.02</v>
       </c>
-      <c r="V3" s="13">
+      <c r="V3" s="9">
         <v>0.01</v>
       </c>
-      <c r="W3" s="13">
+      <c r="W3" s="9">
         <f>((1-U3)/V3^2 -1/U3)*U3^2</f>
         <v>3.9000000000000004</v>
       </c>
-      <c r="X3" s="13">
+      <c r="X3" s="9">
         <f>W3*(1/U3-1)</f>
         <v>191.10000000000002</v>
       </c>
     </row>
     <row r="4" spans="1:24" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7">
+      <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="5">
         <v>1.99</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="5">
         <v>3</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="5">
         <f>LN(E4)</f>
         <v>0.68813463873640102</v>
       </c>
-      <c r="H4" s="7">
+      <c r="H4" s="5">
         <f>(LN(J4)-LN(I4))/(2*NORMINV(0.975,0,1))</f>
         <v>0.2507383667215965</v>
       </c>
-      <c r="I4" s="7">
+      <c r="I4" s="5">
         <v>1.22</v>
       </c>
-      <c r="J4" s="7">
+      <c r="J4" s="5">
         <v>3.26</v>
       </c>
-      <c r="K4" s="7">
+      <c r="K4" s="5">
         <v>2.4781339999999999E-3</v>
       </c>
-      <c r="L4" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="M4" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="T4" s="13"/>
-      <c r="U4" s="13" t="s">
+      <c r="L4" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="T4" s="9"/>
+      <c r="U4" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="V4" s="13" t="s">
+      <c r="V4" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="W4" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="X4" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="W4" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="X4" s="13" t="s">
-        <v>69</v>
-      </c>
     </row>
     <row r="5" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7">
+      <c r="A5" s="5">
         <v>4</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D5" s="7" t="s">
+      <c r="C5" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="5">
         <v>2.04</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="5">
         <v>3</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="5">
         <f>LN(E5)</f>
         <v>0.71294980785612505</v>
       </c>
-      <c r="H5" s="7">
+      <c r="H5" s="5">
         <f t="shared" ref="H5" si="0">(LN(J5)-LN(I5))/(2*NORMINV(0.975,0,1))</f>
         <v>4.9935758684879816E-2</v>
       </c>
-      <c r="I5" s="7">
+      <c r="I5" s="5">
         <v>1.85</v>
       </c>
-      <c r="J5" s="7">
+      <c r="J5" s="5">
         <v>2.25</v>
       </c>
-      <c r="K5" s="7">
+      <c r="K5" s="5">
         <v>6.9413790000000003E-4</v>
       </c>
-      <c r="L5" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="M5" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="T5" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="U5" s="13">
+      <c r="L5" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="T5" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="U5" s="9">
         <v>0.02</v>
       </c>
-      <c r="V5" s="13">
+      <c r="V5" s="9">
         <v>0.01</v>
       </c>
-      <c r="W5" s="13">
+      <c r="W5" s="9">
         <f>U5^2/V5</f>
         <v>0.04</v>
       </c>
-      <c r="X5" s="13">
+      <c r="X5" s="9">
         <f>V5/U5</f>
         <v>0.5</v>
       </c>
     </row>
     <row r="6" spans="1:24" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="7">
+      <c r="A6" s="5">
         <v>5</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="D6" s="7" t="s">
+      <c r="C6" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="5">
         <v>3.47</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="5">
         <v>3</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="5">
         <f>LN(E6)</f>
         <v>1.2441545939587679</v>
       </c>
-      <c r="H6" s="7">
+      <c r="H6" s="5">
         <f>(LN(J6)-LN(I6))/(2*NORMINV(0.975,0,1))</f>
         <v>6.1700065487409E-2</v>
       </c>
-      <c r="I6" s="7">
+      <c r="I6" s="5">
         <v>3.07</v>
       </c>
-      <c r="J6" s="7">
+      <c r="J6" s="5">
         <v>3.91</v>
       </c>
-      <c r="K6" s="7">
+      <c r="K6" s="5">
         <v>1.458268E-3</v>
       </c>
-      <c r="L6" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="M6" s="8" t="s">
-        <v>54</v>
+      <c r="L6" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:24" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="7">
+      <c r="A7" s="5">
         <v>6</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="E7" s="7">
+      <c r="C7" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" s="5">
         <v>1.2</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="5">
         <v>3</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="5">
         <f t="shared" ref="G7:G8" si="1">LN(E7)</f>
         <v>0.18232155679395459</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="5">
         <f t="shared" ref="H7:H8" si="2">(LN(J7)-LN(I7))/(2*NORMINV(0.975,0,1))</f>
         <v>2.5531963685666733E-2</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I7" s="5">
         <v>1.1399999999999999</v>
       </c>
-      <c r="J7" s="7">
+      <c r="J7" s="5">
         <v>1.26</v>
       </c>
-      <c r="K7" s="7"/>
-      <c r="L7" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="M7" s="8" t="s">
-        <v>73</v>
+      <c r="K7" s="5"/>
+      <c r="L7" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="M7" s="6" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:24" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="7">
+      <c r="A8" s="5">
         <v>7</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="E8" s="7">
+      <c r="C8" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E8" s="5">
         <v>2.76</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="5">
         <v>3</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="5">
         <f t="shared" si="1"/>
         <v>1.0152306797290584</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H8" s="5">
         <f t="shared" si="2"/>
         <v>9.2440087521680724E-3</v>
       </c>
-      <c r="I8" s="7">
+      <c r="I8" s="5">
         <v>2.71</v>
       </c>
-      <c r="J8" s="7">
+      <c r="J8" s="5">
         <v>2.81</v>
       </c>
-      <c r="K8" s="7"/>
-      <c r="L8" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="M8" s="8" t="s">
-        <v>73</v>
+      <c r="K8" s="5"/>
+      <c r="L8" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="M8" s="6" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:24" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="7">
+      <c r="A9" s="5">
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -1247,552 +1241,634 @@
       <c r="M9" s="5"/>
     </row>
     <row r="10" spans="1:24" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
+      <c r="A10" s="5">
         <v>9</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="D10" s="7" t="s">
+      <c r="C10" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="5">
         <f>AVERAGE(G10:H10)</f>
         <v>1.0500004999999999</v>
       </c>
-      <c r="F10" s="12">
+      <c r="F10" s="5">
         <v>4</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="5">
         <v>1.0000009999999999</v>
       </c>
-      <c r="H10" s="7">
+      <c r="H10" s="5">
         <v>1.1000000000000001</v>
       </c>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7" t="s">
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="M10" s="9"/>
+      <c r="M10" s="7"/>
     </row>
     <row r="11" spans="1:24" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
+      <c r="A11" s="5">
         <v>10</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="D11" s="7" t="s">
+      <c r="C11" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="5">
         <f>AVERAGE(G11:H11)</f>
         <v>1.25</v>
       </c>
-      <c r="F11" s="12">
+      <c r="F11" s="5">
         <v>4</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="5">
         <v>1</v>
       </c>
-      <c r="H11" s="7">
+      <c r="H11" s="5">
         <v>1.5</v>
       </c>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7" t="s">
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="M11" s="7"/>
+      <c r="M11" s="5"/>
     </row>
     <row r="12" spans="1:24" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="7">
+      <c r="A12" s="5">
         <v>11</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="D12" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="E12" s="7">
+      <c r="E12" s="5">
         <v>0.05</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="5">
         <v>5</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G12" s="5">
         <v>0.05</v>
       </c>
-      <c r="H12" s="7">
+      <c r="H12" s="5">
         <v>0.1</v>
       </c>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7" t="s">
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="M12" s="7"/>
-    </row>
-    <row r="13" spans="1:24" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="7">
+      <c r="M12" s="5"/>
+    </row>
+    <row r="13" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
         <v>12</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E13" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="F13" s="5">
+        <v>5</v>
+      </c>
+      <c r="G13" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="H13" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="M13" s="5"/>
+    </row>
+    <row r="14" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>13</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E14" s="5">
+        <v>1.2</v>
+      </c>
+      <c r="F14" s="5">
+        <v>5</v>
+      </c>
+      <c r="G14" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="H14" s="5">
+        <v>1.7</v>
+      </c>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="M14" s="7"/>
+    </row>
+    <row r="15" spans="1:24" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>11</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E15" s="5">
+        <v>0.95</v>
+      </c>
+      <c r="F15" s="5">
+        <v>4</v>
+      </c>
+      <c r="G15" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="H15" s="5">
+        <v>1</v>
+      </c>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="M15" s="5"/>
+    </row>
+    <row r="16" spans="1:24" ht="75" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>12</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="D13" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="E13" s="7">
-        <v>0.1</v>
-      </c>
-      <c r="F13" s="7">
-        <v>5</v>
-      </c>
-      <c r="G13" s="7">
-        <v>0.01</v>
-      </c>
-      <c r="H13" s="7">
-        <v>0.2</v>
-      </c>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="M13" s="7"/>
-    </row>
-    <row r="14" spans="1:24" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="7">
-        <v>13</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="8" t="s">
+      <c r="D16" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="D14" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="E14" s="7">
-        <v>1.2</v>
-      </c>
-      <c r="F14">
-        <v>5</v>
-      </c>
-      <c r="G14" s="7">
-        <v>1.01</v>
-      </c>
-      <c r="H14" s="7">
-        <v>1.7</v>
-      </c>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="M14" s="9"/>
-    </row>
-    <row r="15" spans="1:24" ht="75" x14ac:dyDescent="0.25">
-      <c r="A15" s="7">
-        <v>11</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="E15" s="7">
-        <v>-5.0000000000000001E-3</v>
-      </c>
-      <c r="F15" s="7">
-        <v>5</v>
-      </c>
-      <c r="G15" s="7">
-        <v>-5.0000000000000001E-3</v>
-      </c>
-      <c r="H15" s="7">
-        <v>0.2</v>
-      </c>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="M15" s="7"/>
-    </row>
-    <row r="16" spans="1:24" ht="75" x14ac:dyDescent="0.25">
-      <c r="A16" s="7">
-        <v>12</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="E16" s="7">
+      <c r="E16" s="5">
         <f>AVERAGE(G16:H16)</f>
         <v>-5.5E-2</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F16" s="5">
         <v>4</v>
       </c>
-      <c r="G16" s="7">
+      <c r="G16" s="5">
         <v>-0.1</v>
       </c>
-      <c r="H16" s="7">
+      <c r="H16" s="5">
         <v>-0.01</v>
       </c>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7" t="s">
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="M16" s="7"/>
+      <c r="M16" s="5"/>
     </row>
     <row r="17" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
-      <c r="B17" s="12" t="s">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="E17" s="5">
+        <v>3</v>
+      </c>
+      <c r="F17" s="5">
+        <v>6</v>
+      </c>
+      <c r="G17" s="5">
+        <v>3</v>
+      </c>
+      <c r="H17" s="5">
+        <v>3</v>
+      </c>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="M17" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
+        <v>14</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="E18" s="5">
+        <v>2</v>
+      </c>
+      <c r="F18" s="5">
+        <v>6</v>
+      </c>
+      <c r="G18" s="5">
+        <v>2</v>
+      </c>
+      <c r="H18" s="5">
+        <v>2</v>
+      </c>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="M18" s="5"/>
+    </row>
+    <row r="19" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>15</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E19" s="5">
+        <v>1</v>
+      </c>
+      <c r="F19" s="5">
+        <v>6</v>
+      </c>
+      <c r="G19" s="5">
+        <v>1</v>
+      </c>
+      <c r="H19" s="5">
+        <v>1</v>
+      </c>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="M19" s="8"/>
+    </row>
+    <row r="20" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>16</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="D17" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="E17" s="7">
-        <v>3</v>
-      </c>
-      <c r="F17" s="7">
+      <c r="D20" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E20" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="F20" s="5">
         <v>6</v>
       </c>
-      <c r="G17" s="7">
-        <v>3</v>
-      </c>
-      <c r="H17" s="7">
-        <v>3</v>
-      </c>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="M17" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="7">
-        <v>14</v>
-      </c>
-      <c r="B18" s="12" t="s">
+      <c r="G20" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="H20" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="M20" s="5"/>
+    </row>
+    <row r="21" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>17</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="D18" s="7" t="s">
+      <c r="C21" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E21" s="5">
+        <v>1.0009999999999999</v>
+      </c>
+      <c r="F21" s="5">
+        <v>4</v>
+      </c>
+      <c r="G21" s="5">
+        <v>1.0009999999999999</v>
+      </c>
+      <c r="H21" s="5">
+        <v>1.2</v>
+      </c>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="M21" s="6"/>
+    </row>
+    <row r="22" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
+        <v>18</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="E18" s="7">
-        <v>2</v>
-      </c>
-      <c r="F18" s="7">
+      <c r="E22" s="5">
+        <v>1.0009999999999999</v>
+      </c>
+      <c r="F22" s="5">
+        <v>4</v>
+      </c>
+      <c r="G22" s="5">
+        <v>1.0009999999999999</v>
+      </c>
+      <c r="H22" s="5">
+        <v>1.2</v>
+      </c>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="M22" s="5"/>
+    </row>
+    <row r="23" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
+        <v>19</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="E23" s="5">
+        <v>1.0009999999999999</v>
+      </c>
+      <c r="F23" s="5">
+        <v>4</v>
+      </c>
+      <c r="G23" s="5">
+        <v>1.0009999999999999</v>
+      </c>
+      <c r="H23" s="5">
+        <v>1.2</v>
+      </c>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="M23" s="5"/>
+    </row>
+    <row r="24" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
+        <v>20</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="E24" s="5">
+        <v>4.7999999999999996E-3</v>
+      </c>
+      <c r="F24" s="5">
         <v>6</v>
       </c>
-      <c r="G18" s="7">
-        <v>2</v>
-      </c>
-      <c r="H18" s="7">
-        <v>2</v>
-      </c>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="M18" s="7"/>
-    </row>
-    <row r="19" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="7">
-        <v>15</v>
-      </c>
-      <c r="B19" s="12" t="s">
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="M24" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
+        <v>21</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="E19" s="7">
-        <v>1</v>
-      </c>
-      <c r="F19" s="12">
-        <v>6</v>
-      </c>
-      <c r="G19" s="7">
-        <v>1</v>
-      </c>
-      <c r="H19" s="7">
-        <v>1</v>
-      </c>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="M19" s="10"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="7"/>
-      <c r="M20" s="7"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7"/>
-      <c r="M21" s="8"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
-      <c r="K22" s="7"/>
-      <c r="L22" s="7"/>
-      <c r="M22" s="7"/>
-    </row>
-    <row r="23" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C23" s="8" t="s">
+      <c r="C25" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E25" s="5">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="F25" s="5">
+        <v>5</v>
+      </c>
+      <c r="G25" s="5">
+        <f>E25</f>
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="H25" s="5">
+        <f>(J25-I25)/(2*NORMINV(0.975,0,1))</f>
+        <v>1.6837044078513583E-2</v>
+      </c>
+      <c r="I25" s="5">
+        <v>0.253</v>
+      </c>
+      <c r="J25" s="5">
+        <v>0.31900000000000001</v>
+      </c>
+      <c r="K25" s="5"/>
+      <c r="L25" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="M25" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D23" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="E23" s="11"/>
-      <c r="F23" s="12">
-        <v>2</v>
-      </c>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="7"/>
-      <c r="L23" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="M23" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7">
-        <v>0</v>
-      </c>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7">
-        <v>0</v>
-      </c>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7">
-        <v>0</v>
-      </c>
-      <c r="J24" s="7"/>
-      <c r="K24" s="7"/>
-      <c r="L24" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="M24" s="7"/>
-    </row>
-    <row r="25" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
-      <c r="B25" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="7"/>
-      <c r="K25" s="7"/>
-      <c r="L25" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="M25" s="8" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="7"/>
-      <c r="J26" s="7"/>
-      <c r="K26" s="7"/>
-      <c r="L26" s="7"/>
-      <c r="M26" s="7"/>
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="M26" s="5"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="7"/>
-      <c r="J27" s="7"/>
-      <c r="K27" s="7"/>
-      <c r="L27" s="7"/>
-      <c r="M27" s="7"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="5"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="5"/>
-      <c r="L29" s="5"/>
-      <c r="M29" s="5"/>
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
+    </row>
+    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M33">
+        <v>12</v>
+      </c>
+      <c r="N33">
+        <f>M33*N34/M34</f>
+        <v>0.47213114754098356</v>
+      </c>
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.25">
       <c r="M34">
-        <v>12</v>
+        <v>61</v>
       </c>
       <c r="N34">
-        <f>M34*N35/M35</f>
-        <v>0.47213114754098356</v>
-      </c>
-    </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="M35">
-        <v>61</v>
-      </c>
-      <c r="N35">
         <v>2.4</v>
       </c>
     </row>
-    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
+    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
         <v>38</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C38" t="s">
         <v>39</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D38" t="s">
         <v>40</v>
       </c>
-      <c r="E39">
+      <c r="E38">
         <v>4.3199999999999992E-3</v>
       </c>
-      <c r="G39">
-        <f>E39</f>
+      <c r="G38">
+        <f>E38</f>
         <v>4.3199999999999992E-3</v>
       </c>
-      <c r="H39">
-        <f>(J39-I39)/(2*NORMINV(0.975,0,1))</f>
+      <c r="H38">
+        <f>(J38-I38)/(2*NORMINV(0.975,0,1))</f>
         <v>1.4285976793890307E-4</v>
       </c>
-      <c r="I39">
+      <c r="I38">
         <v>4.0400000000000002E-3</v>
       </c>
-      <c r="J39">
+      <c r="J38">
         <v>4.5999999999999999E-3</v>
       </c>
-      <c r="L39" t="s">
+      <c r="L38" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1812,10 +1888,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F32D2E0-32A8-4C75-8C98-9C12E5C1268D}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1828,7 +1904,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>4</v>
@@ -1837,355 +1913,355 @@
         <v>9</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="B2" s="17">
+      <c r="A2" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="11">
         <f>parameters!E2</f>
         <v>1E-4</v>
       </c>
-      <c r="C2" s="17">
+      <c r="C2" s="11">
         <f>parameters!F2</f>
         <v>1</v>
       </c>
-      <c r="D2" s="17">
+      <c r="D2" s="11">
         <f>parameters!G2</f>
         <v>0.99980000000000002</v>
       </c>
-      <c r="E2" s="17">
+      <c r="E2" s="11">
         <f>parameters!H2</f>
         <v>9997.0002000000004</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="17">
+      <c r="B3" s="11">
         <f>parameters!E3</f>
         <v>0.192</v>
       </c>
-      <c r="C3" s="17">
+      <c r="C3" s="11">
         <f>parameters!F3</f>
         <v>1</v>
       </c>
-      <c r="D3" s="17">
+      <c r="D3" s="11">
         <f>parameters!G3</f>
         <v>4765.5859199999986</v>
       </c>
-      <c r="E3" s="17">
+      <c r="E3" s="11">
         <f>parameters!H3</f>
         <v>20055.174079999993</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="17">
+      <c r="B4" s="11">
         <f>parameters!E4</f>
         <v>1.99</v>
       </c>
-      <c r="C4" s="17">
+      <c r="C4" s="11">
         <f>parameters!F4</f>
         <v>3</v>
       </c>
-      <c r="D4" s="17">
+      <c r="D4" s="11">
         <f>parameters!G4</f>
         <v>0.68813463873640102</v>
       </c>
-      <c r="E4" s="17">
+      <c r="E4" s="11">
         <f>parameters!H4</f>
         <v>0.2507383667215965</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="17">
+      <c r="B5" s="11">
         <f>parameters!E5</f>
         <v>2.04</v>
       </c>
-      <c r="C5" s="17">
+      <c r="C5" s="11">
         <f>parameters!F5</f>
         <v>3</v>
       </c>
-      <c r="D5" s="17">
+      <c r="D5" s="11">
         <f>parameters!G5</f>
         <v>0.71294980785612505</v>
       </c>
-      <c r="E5" s="17">
+      <c r="E5" s="11">
         <f>parameters!H5</f>
         <v>4.9935758684879816E-2</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="17">
+      <c r="B6" s="11">
         <f>parameters!E6</f>
         <v>3.47</v>
       </c>
-      <c r="C6" s="17">
+      <c r="C6" s="11">
         <f>parameters!F6</f>
         <v>3</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6" s="11">
         <f>parameters!G6</f>
         <v>1.2441545939587679</v>
       </c>
-      <c r="E6" s="17">
+      <c r="E6" s="11">
         <f>parameters!H6</f>
         <v>6.1700065487409E-2</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="str">
+      <c r="A7" s="11" t="str">
         <f>parameters!D7</f>
         <v>RR.All.Death.past_smoke</v>
       </c>
-      <c r="B7" s="17">
+      <c r="B7" s="11">
         <f>parameters!E7</f>
         <v>1.2</v>
       </c>
-      <c r="C7" s="17">
+      <c r="C7" s="11">
         <f>parameters!F7</f>
         <v>3</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="11">
         <f>parameters!G7</f>
         <v>0.18232155679395459</v>
       </c>
-      <c r="E7" s="17">
+      <c r="E7" s="11">
         <f>parameters!H7</f>
         <v>2.5531963685666733E-2</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="str">
+      <c r="A8" s="11" t="str">
         <f>parameters!D8</f>
         <v>RR.All.Death.current_smoke</v>
       </c>
-      <c r="B8" s="17">
+      <c r="B8" s="11">
         <f>parameters!E8</f>
         <v>2.76</v>
       </c>
-      <c r="C8" s="17">
+      <c r="C8" s="11">
         <f>parameters!F8</f>
         <v>3</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D8" s="11">
         <f>parameters!G8</f>
         <v>1.0152306797290584</v>
       </c>
-      <c r="E8" s="17">
+      <c r="E8" s="11">
         <f>parameters!H8</f>
         <v>9.2440087521680724E-3</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="str">
+      <c r="A9" s="11" t="str">
         <f>parameters!D9</f>
         <v>P.quit.smoke</v>
       </c>
-      <c r="B9" s="17">
+      <c r="B9" s="11">
         <f>parameters!E9</f>
         <v>1.67E-2</v>
       </c>
-      <c r="C9" s="17">
+      <c r="C9" s="11">
         <f>parameters!F9</f>
         <v>5</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9" s="11">
         <f>parameters!G9</f>
         <v>1.67E-2</v>
       </c>
-      <c r="E9" s="17">
+      <c r="E9" s="11">
         <f>parameters!H9</f>
         <v>4.0523713428230627E-4</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="str">
+      <c r="A10" s="11" t="str">
         <f>parameters!D10</f>
         <v>P.onset_age</v>
       </c>
-      <c r="B10" s="17">
+      <c r="B10" s="11">
         <f>parameters!E10</f>
         <v>1.0500004999999999</v>
       </c>
-      <c r="C10" s="17">
+      <c r="C10" s="11">
         <f>parameters!F10</f>
         <v>4</v>
       </c>
-      <c r="D10" s="17">
+      <c r="D10" s="11">
         <f>parameters!G10</f>
         <v>1.0000009999999999</v>
       </c>
-      <c r="E10" s="17">
+      <c r="E10" s="11">
         <f>parameters!H10</f>
         <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="str">
+      <c r="A11" s="11" t="str">
         <f>parameters!D11</f>
         <v>P.onset_sex</v>
       </c>
-      <c r="B11" s="17">
+      <c r="B11" s="11">
         <f>parameters!E11</f>
         <v>1.25</v>
       </c>
-      <c r="C11" s="17">
+      <c r="C11" s="11">
         <f>parameters!F11</f>
         <v>4</v>
       </c>
-      <c r="D11" s="17">
+      <c r="D11" s="11">
         <f>parameters!G11</f>
         <v>1</v>
       </c>
-      <c r="E11" s="17">
+      <c r="E11" s="11">
         <f>parameters!H11</f>
         <v>1.5</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="17" t="str">
+      <c r="A12" s="11" t="str">
         <f>parameters!D12</f>
         <v>P.sympt.diag_LGBC</v>
       </c>
-      <c r="B12" s="17">
+      <c r="B12" s="11">
         <f>parameters!E12</f>
         <v>0.05</v>
       </c>
-      <c r="C12" s="17">
+      <c r="C12" s="11">
         <f>parameters!F12</f>
         <v>5</v>
       </c>
-      <c r="D12" s="17">
+      <c r="D12" s="11">
         <f>parameters!G12</f>
         <v>0.05</v>
       </c>
-      <c r="E12" s="17">
+      <c r="E12" s="11">
         <f>parameters!H12</f>
         <v>0.1</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="str">
+      <c r="A13" s="11" t="str">
         <f>parameters!D13</f>
         <v>P.sympt.diag_A_HGBC</v>
       </c>
-      <c r="B13" s="17">
+      <c r="B13" s="11">
         <f>parameters!E13</f>
         <v>0.1</v>
       </c>
-      <c r="C13" s="17">
+      <c r="C13" s="11">
         <f>parameters!F13</f>
         <v>5</v>
       </c>
-      <c r="D13" s="17">
+      <c r="D13" s="11">
         <f>parameters!G13</f>
         <v>0.01</v>
       </c>
-      <c r="E13" s="17">
+      <c r="E13" s="11">
         <f>parameters!H13</f>
         <v>0.2</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="17" t="str">
+      <c r="A14" s="11" t="str">
         <f>parameters!D14</f>
         <v>P.sympt.diag_B_HGBC</v>
       </c>
-      <c r="B14" s="17">
+      <c r="B14" s="11">
         <f>parameters!E14</f>
         <v>1.2</v>
       </c>
-      <c r="C14" s="17">
+      <c r="C14" s="11">
         <f>parameters!F14</f>
         <v>5</v>
       </c>
-      <c r="D14" s="17">
+      <c r="D14" s="11">
         <f>parameters!G14</f>
         <v>1.01</v>
       </c>
-      <c r="E14" s="17">
+      <c r="E14" s="11">
         <f>parameters!H14</f>
         <v>1.7</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="str">
+      <c r="A15" s="11" t="str">
         <f>parameters!D15</f>
         <v>P.sympt.diag_Age80_HGBC</v>
       </c>
-      <c r="B15" s="17">
+      <c r="B15" s="11">
         <f>parameters!E15</f>
-        <v>-5.0000000000000001E-3</v>
-      </c>
-      <c r="C15" s="17">
+        <v>0.95</v>
+      </c>
+      <c r="C15" s="11">
         <f>parameters!F15</f>
-        <v>5</v>
-      </c>
-      <c r="D15" s="17">
+        <v>4</v>
+      </c>
+      <c r="D15" s="11">
         <f>parameters!G15</f>
-        <v>-5.0000000000000001E-3</v>
-      </c>
-      <c r="E15" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="E15" s="11">
         <f>parameters!H15</f>
-        <v>0.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="str">
+      <c r="A16" s="11" t="str">
         <f>parameters!D16</f>
         <v>C.age.80.undiag.mort</v>
       </c>
-      <c r="B16" s="17">
+      <c r="B16" s="11">
         <f>parameters!E16</f>
         <v>-5.5E-2</v>
       </c>
-      <c r="C16" s="17">
+      <c r="C16" s="11">
         <f>parameters!F16</f>
         <v>4</v>
       </c>
-      <c r="D16" s="17">
+      <c r="D16" s="11">
         <f>parameters!G16</f>
         <v>-0.1</v>
       </c>
-      <c r="E16" s="17">
+      <c r="E16" s="11">
         <f>parameters!H16</f>
         <v>-0.01</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="str">
+      <c r="A17" s="11" t="str">
         <f>parameters!D17</f>
         <v>Mean.t.StI.StII</v>
       </c>
-      <c r="B17" s="17">
+      <c r="B17" s="11">
         <f>parameters!E17</f>
         <v>3</v>
       </c>
-      <c r="C17" s="17">
+      <c r="C17" s="11">
         <f>parameters!F17</f>
         <v>6</v>
       </c>
-      <c r="D17" s="17">
+      <c r="D17" s="11">
         <f>parameters!G17</f>
         <v>3</v>
       </c>
-      <c r="E17" s="17">
+      <c r="E17" s="11">
         <f>parameters!H17</f>
         <v>3</v>
       </c>
@@ -2232,6 +2308,138 @@
       <c r="E19">
         <f>parameters!H19</f>
         <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="str">
+        <f>parameters!D20</f>
+        <v>RR.All.Death.no_smoke</v>
+      </c>
+      <c r="B20">
+        <f>parameters!E20</f>
+        <v>0.8</v>
+      </c>
+      <c r="C20">
+        <f>parameters!F20</f>
+        <v>6</v>
+      </c>
+      <c r="D20">
+        <f>parameters!G20</f>
+        <v>0.8</v>
+      </c>
+      <c r="E20">
+        <f>parameters!H20</f>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="str">
+        <f>parameters!D21</f>
+        <v>shape.t.StI.StII</v>
+      </c>
+      <c r="B21">
+        <f>parameters!E21</f>
+        <v>1.0009999999999999</v>
+      </c>
+      <c r="C21">
+        <f>parameters!F21</f>
+        <v>4</v>
+      </c>
+      <c r="D21">
+        <f>parameters!G21</f>
+        <v>1.0009999999999999</v>
+      </c>
+      <c r="E21">
+        <f>parameters!H21</f>
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="str">
+        <f>parameters!D22</f>
+        <v>shape.t.StII.StIII</v>
+      </c>
+      <c r="B22">
+        <f>parameters!E22</f>
+        <v>1.0009999999999999</v>
+      </c>
+      <c r="C22">
+        <f>parameters!F22</f>
+        <v>4</v>
+      </c>
+      <c r="D22">
+        <f>parameters!G22</f>
+        <v>1.0009999999999999</v>
+      </c>
+      <c r="E22">
+        <f>parameters!H22</f>
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="str">
+        <f>parameters!D23</f>
+        <v>shape.t.StIII.StIV</v>
+      </c>
+      <c r="B23">
+        <f>parameters!E23</f>
+        <v>1.0009999999999999</v>
+      </c>
+      <c r="C23">
+        <f>parameters!F23</f>
+        <v>4</v>
+      </c>
+      <c r="D23">
+        <f>parameters!G23</f>
+        <v>1.0009999999999999</v>
+      </c>
+      <c r="E23">
+        <f>parameters!H23</f>
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="str">
+        <f>parameters!D24</f>
+        <v>P.LGtoHGBC</v>
+      </c>
+      <c r="B24">
+        <f>parameters!E24</f>
+        <v>4.7999999999999996E-3</v>
+      </c>
+      <c r="C24">
+        <f>parameters!F24</f>
+        <v>6</v>
+      </c>
+      <c r="D24">
+        <f>parameters!G24</f>
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <f>parameters!H24</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="str">
+        <f>parameters!D25</f>
+        <v>P.Recurrence.LR</v>
+      </c>
+      <c r="B25">
+        <f>parameters!E25</f>
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="C25">
+        <f>parameters!F25</f>
+        <v>5</v>
+      </c>
+      <c r="D25">
+        <f>parameters!G25</f>
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="E25">
+        <f>parameters!H25</f>
+        <v>1.6837044078513583E-2</v>
       </c>
     </row>
   </sheetData>
@@ -2314,10 +2522,10 @@
     </row>
     <row r="6" spans="2:26" x14ac:dyDescent="0.25">
       <c r="L6" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="M6" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="2:26" x14ac:dyDescent="0.25">
@@ -2334,7 +2542,7 @@
         <v>25</v>
       </c>
       <c r="K7" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="L7">
         <v>1.01</v>
@@ -2380,7 +2588,7 @@
         <v>0.10100000000000001</v>
       </c>
       <c r="P9" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="2:26" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Addressed comments on internal validation
</commit_message>
<xml_diff>
--- a/Parameters bladder cancer model.xlsx
+++ b/Parameters bladder cancer model.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cm1om\Documents\Research\Cancer\Bladder\Bladder_cancer_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{499BE5F9-49B8-4B52-ADDF-8BB3B6AD8112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCDBF54A-0E84-4E35-B0A2-87027C03567D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1AD6D928-CCB7-482A-A47C-26785A7D3A52}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1AD6D928-CCB7-482A-A47C-26785A7D3A52}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
     <sheet name="extract" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId3"/>
+    <sheet name="sensitivity" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="126">
   <si>
     <t>Param number</t>
   </si>
@@ -120,9 +121,6 @@
   </si>
   <si>
     <t>P.onset_age</t>
-  </si>
-  <si>
-    <t>P.onset_sex</t>
   </si>
   <si>
     <t>P.onset_low.risk</t>
@@ -356,13 +354,77 @@
   </si>
   <si>
     <t>P.LGtoHGBC</t>
+  </si>
+  <si>
+    <t>Natural History</t>
+  </si>
+  <si>
+    <t>Test accuracy</t>
+  </si>
+  <si>
+    <t>Specificity haematuria dipstick (hom)</t>
+  </si>
+  <si>
+    <t>Sensitivity for CT + cystoscopy +TURBT (follow up screen positive)</t>
+  </si>
+  <si>
+    <t>Specificity for CT + cystoscopy +TURBT (follow up screen positive)</t>
+  </si>
+  <si>
+    <t>Mortality rate of TURBT</t>
+  </si>
+  <si>
+    <t>Kondas J, Szentgyorgyi E. Transurethral resection of 1250 bladder tumours. International urology and
+nephrology. 1992; 24(1):35–42. PMID: 1378046.</t>
+  </si>
+  <si>
+    <t>Used in Staton et al (2018)</t>
+  </si>
+  <si>
+    <t>Nicolau, C (2011)</t>
+  </si>
+  <si>
+    <t>The Roche Combur 5 HC test</t>
+  </si>
+  <si>
+    <t>Sensitivity haematuria dipstick (home) to LG cancers</t>
+  </si>
+  <si>
+    <t>Saad (2002)</t>
+  </si>
+  <si>
+    <t>https://bjui-journals.onlinelibrary.wiley.com/doi/full/10.1046/j.1464-4096.2001.01699.x?casa_token=OVG-kOzIWF4AAAAA%3AtwaUeAuNMdlpbnodfcPI_iuRs8-a3tUBVMWWcMB7xudPxbPrELkjGKZtvT1k9DwLohoRs7nJ6D6e</t>
+  </si>
+  <si>
+    <t>Sensitivity haematuria dipstick (home) to HG Stage 1 BC</t>
+  </si>
+  <si>
+    <t>Assumed to be = Sensitivity to G1 cancers</t>
+  </si>
+  <si>
+    <t>Assumed to be = Sensitivity to sensitivity pT1 and G2 cancers</t>
+  </si>
+  <si>
+    <t>Assumed to be = Sensitivity to pT2 cancers</t>
+  </si>
+  <si>
+    <t>Sensitivity haematuria dipstick (home) to HG Stage 2 BC</t>
+  </si>
+  <si>
+    <t>Sensitivity haematuria dipstick (home) to HG Stage 3,4 BC</t>
+  </si>
+  <si>
+    <t>Assumption based on Boman et al (2002)</t>
+  </si>
+  <si>
+    <t>RR.onset_sex</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -400,8 +462,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -426,6 +502,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -440,7 +534,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -465,6 +559,25 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -786,16 +899,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8694223C-410D-4023-9128-3FD5F8A481E4}">
-  <dimension ref="A1:X38"/>
+  <dimension ref="A1:X41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="9.5703125" customWidth="1"/>
-    <col min="3" max="3" width="43.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="60.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.28515625" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
@@ -827,14 +940,14 @@
       <c r="F1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="12"/>
-      <c r="I1" s="13" t="s">
+      <c r="H1" s="21"/>
+      <c r="I1" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="13"/>
+      <c r="J1" s="22"/>
       <c r="K1" s="2" t="s">
         <v>7</v>
       </c>
@@ -845,460 +958,442 @@
         <v>12</v>
       </c>
       <c r="O1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="16"/>
+    </row>
+    <row r="3" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
         <v>1</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="E2" s="5">
-        <v>1E-4</v>
-      </c>
-      <c r="F2" s="5">
-        <v>1</v>
-      </c>
-      <c r="G2" s="5">
-        <f>((1-E2)/(K2^2)^2 -1/E2)*E2^2</f>
-        <v>0.99980000000000002</v>
-      </c>
-      <c r="H2" s="5">
-        <f>G2*(1/E2-1)</f>
-        <v>9997.0002000000004</v>
-      </c>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5">
-        <v>0.01</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M2" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="T2" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="U2" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="V2" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="W2" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="X2" s="9" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
-        <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="E3" s="5">
-        <v>0.192</v>
+        <v>1E-4</v>
       </c>
       <c r="F3" s="5">
         <v>1</v>
       </c>
       <c r="G3" s="5">
         <f>((1-E3)/(K3^2)^2 -1/E3)*E3^2</f>
-        <v>4765.5859199999986</v>
+        <v>0.99980000000000002</v>
       </c>
       <c r="H3" s="5">
         <f>G3*(1/E3-1)</f>
-        <v>20055.174079999993</v>
+        <v>9997.0002000000004</v>
       </c>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
       <c r="K3" s="5">
-        <v>0.05</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>51</v>
+        <v>0.01</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="T3" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="U3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="V3" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="U3" s="9">
-        <v>0.02</v>
-      </c>
-      <c r="V3" s="9">
-        <v>0.01</v>
-      </c>
-      <c r="W3" s="9">
-        <f>((1-U3)/V3^2 -1/U3)*U3^2</f>
-        <v>3.9000000000000004</v>
-      </c>
-      <c r="X3" s="9">
-        <f>W3*(1/U3-1)</f>
-        <v>191.10000000000002</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W3" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="X3" s="9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E4" s="5">
-        <v>1.99</v>
+        <v>0.192</v>
       </c>
       <c r="F4" s="5">
+        <v>1</v>
+      </c>
+      <c r="G4" s="5">
+        <f>((1-E4)/(K4^2)^2 -1/E4)*E4^2</f>
+        <v>4765.5859199999986</v>
+      </c>
+      <c r="H4" s="5">
+        <f>G4*(1/E4-1)</f>
+        <v>20055.174079999993</v>
+      </c>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="M4" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="T4" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="U4" s="9">
+        <v>0.02</v>
+      </c>
+      <c r="V4" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="W4" s="9">
+        <f>((1-U4)/V4^2 -1/U4)*U4^2</f>
+        <v>3.9000000000000004</v>
+      </c>
+      <c r="X4" s="9">
+        <f>W4*(1/U4-1)</f>
+        <v>191.10000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
         <v>3</v>
-      </c>
-      <c r="G4" s="5">
-        <f>LN(E4)</f>
-        <v>0.68813463873640102</v>
-      </c>
-      <c r="H4" s="5">
-        <f>(LN(J4)-LN(I4))/(2*NORMINV(0.975,0,1))</f>
-        <v>0.2507383667215965</v>
-      </c>
-      <c r="I4" s="5">
-        <v>1.22</v>
-      </c>
-      <c r="J4" s="5">
-        <v>3.26</v>
-      </c>
-      <c r="K4" s="5">
-        <v>2.4781339999999999E-3</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="M4" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="T4" s="9"/>
-      <c r="U4" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="V4" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="W4" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="X4" s="9" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
-        <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>53</v>
+        <v>13</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>31</v>
       </c>
       <c r="E5" s="5">
-        <v>2.04</v>
+        <v>1.99</v>
       </c>
       <c r="F5" s="5">
         <v>3</v>
       </c>
       <c r="G5" s="5">
         <f>LN(E5)</f>
-        <v>0.71294980785612505</v>
+        <v>0.68813463873640102</v>
       </c>
       <c r="H5" s="5">
-        <f t="shared" ref="H5" si="0">(LN(J5)-LN(I5))/(2*NORMINV(0.975,0,1))</f>
-        <v>4.9935758684879816E-2</v>
+        <f>(LN(J5)-LN(I5))/(2*NORMINV(0.975,0,1))</f>
+        <v>0.2507383667215965</v>
       </c>
       <c r="I5" s="5">
-        <v>1.85</v>
+        <v>1.22</v>
       </c>
       <c r="J5" s="5">
-        <v>2.25</v>
+        <v>3.26</v>
       </c>
       <c r="K5" s="5">
-        <v>6.9413790000000003E-4</v>
+        <v>2.4781339999999999E-3</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="T5" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="T5" s="9"/>
+      <c r="U5" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="V5" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="W5" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="U5" s="9">
-        <v>0.02</v>
-      </c>
-      <c r="V5" s="9">
-        <v>0.01</v>
-      </c>
-      <c r="W5" s="9">
-        <f>U5^2/V5</f>
-        <v>0.04</v>
-      </c>
-      <c r="X5" s="9">
-        <f>V5/U5</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X5" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>30</v>
       </c>
       <c r="E6" s="5">
-        <v>3.47</v>
+        <v>2.04</v>
       </c>
       <c r="F6" s="5">
         <v>3</v>
       </c>
       <c r="G6" s="5">
         <f>LN(E6)</f>
-        <v>1.2441545939587679</v>
+        <v>0.71294980785612505</v>
       </c>
       <c r="H6" s="5">
-        <f>(LN(J6)-LN(I6))/(2*NORMINV(0.975,0,1))</f>
-        <v>6.1700065487409E-2</v>
+        <f t="shared" ref="H6" si="0">(LN(J6)-LN(I6))/(2*NORMINV(0.975,0,1))</f>
+        <v>4.9935758684879816E-2</v>
       </c>
       <c r="I6" s="5">
-        <v>3.07</v>
+        <v>1.85</v>
       </c>
       <c r="J6" s="5">
-        <v>3.91</v>
+        <v>2.25</v>
       </c>
       <c r="K6" s="5">
-        <v>1.458268E-3</v>
+        <v>6.9413790000000003E-4</v>
       </c>
       <c r="L6" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="M6" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="M6" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+      <c r="T6" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="U6" s="9">
+        <v>0.02</v>
+      </c>
+      <c r="V6" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="W6" s="9">
+        <f>U6^2/V6</f>
+        <v>0.04</v>
+      </c>
+      <c r="X6" s="9">
+        <f>V6/U6</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>67</v>
+        <v>29</v>
       </c>
       <c r="E7" s="5">
-        <v>1.2</v>
+        <v>3.47</v>
       </c>
       <c r="F7" s="5">
         <v>3</v>
       </c>
       <c r="G7" s="5">
-        <f t="shared" ref="G7:G8" si="1">LN(E7)</f>
-        <v>0.18232155679395459</v>
+        <f>LN(E7)</f>
+        <v>1.2441545939587679</v>
       </c>
       <c r="H7" s="5">
-        <f t="shared" ref="H7:H8" si="2">(LN(J7)-LN(I7))/(2*NORMINV(0.975,0,1))</f>
-        <v>2.5531963685666733E-2</v>
+        <f>(LN(J7)-LN(I7))/(2*NORMINV(0.975,0,1))</f>
+        <v>6.1700065487409E-2</v>
       </c>
       <c r="I7" s="5">
-        <v>1.1399999999999999</v>
+        <v>3.07</v>
       </c>
       <c r="J7" s="5">
-        <v>1.26</v>
-      </c>
-      <c r="K7" s="5"/>
-      <c r="L7" s="10" t="s">
-        <v>69</v>
+        <v>3.91</v>
+      </c>
+      <c r="K7" s="5">
+        <v>1.458268E-3</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E8" s="5">
-        <v>2.76</v>
+        <v>1.2</v>
       </c>
       <c r="F8" s="5">
         <v>3</v>
       </c>
       <c r="G8" s="5">
+        <f t="shared" ref="G8:G9" si="1">LN(E8)</f>
+        <v>0.18232155679395459</v>
+      </c>
+      <c r="H8" s="5">
+        <f t="shared" ref="H8:H9" si="2">(LN(J8)-LN(I8))/(2*NORMINV(0.975,0,1))</f>
+        <v>2.5531963685666733E-2</v>
+      </c>
+      <c r="I8" s="5">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="J8" s="5">
+        <v>1.26</v>
+      </c>
+      <c r="K8" s="5"/>
+      <c r="L8" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="M8" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>7</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E9" s="5">
+        <v>2.76</v>
+      </c>
+      <c r="F9" s="5">
+        <v>3</v>
+      </c>
+      <c r="G9" s="5">
         <f t="shared" si="1"/>
         <v>1.0152306797290584</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H9" s="5">
         <f t="shared" si="2"/>
         <v>9.2440087521680724E-3</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I9" s="5">
         <v>2.71</v>
       </c>
-      <c r="J8" s="5">
+      <c r="J9" s="5">
         <v>2.81</v>
       </c>
-      <c r="K8" s="5"/>
-      <c r="L8" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="M8" s="6" t="s">
+      <c r="K9" s="5"/>
+      <c r="L9" s="10" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="9" spans="1:24" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
+      <c r="M9" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
         <v>8</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" s="6" t="s">
+      <c r="B10" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="E10" s="5">
+        <v>1.67E-2</v>
+      </c>
+      <c r="F10" s="5">
+        <v>5</v>
+      </c>
+      <c r="G10" s="5">
+        <f>E10</f>
+        <v>1.67E-2</v>
+      </c>
+      <c r="H10" s="5">
+        <f>(J10-I10)/(2*NORMINV(0.975,0,1))</f>
+        <v>4.0523713428230627E-4</v>
+      </c>
+      <c r="I10" s="5">
+        <f>G10-1.96*SQRT(G10*(1-G10)/100000)</f>
+        <v>1.5905749811608458E-2</v>
+      </c>
+      <c r="J10" s="5">
+        <f>G10+1.96*SQRT(G10*(1-G10)/100000)</f>
+        <v>1.7494250188391541E-2</v>
+      </c>
+      <c r="K10" s="5"/>
+      <c r="L10" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="5">
-        <v>1.67E-2</v>
-      </c>
-      <c r="F9" s="5">
-        <v>5</v>
-      </c>
-      <c r="G9" s="5">
-        <f>E9</f>
-        <v>1.67E-2</v>
-      </c>
-      <c r="H9" s="5">
-        <f>(J9-I9)/(2*NORMINV(0.975,0,1))</f>
-        <v>4.0523713428230627E-4</v>
-      </c>
-      <c r="I9" s="5">
-        <f>G9-1.96*SQRT(G9*(1-G9)/100000)</f>
-        <v>1.5905749811608458E-2</v>
-      </c>
-      <c r="J9" s="5">
-        <f>G9+1.96*SQRT(G9*(1-G9)/100000)</f>
-        <v>1.7494250188391541E-2</v>
-      </c>
-      <c r="K9" s="5"/>
-      <c r="L9" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="M9" s="5"/>
-    </row>
-    <row r="10" spans="1:24" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
+      <c r="M10" s="5"/>
+    </row>
+    <row r="11" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
         <v>9</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" s="5">
-        <f>AVERAGE(G10:H10)</f>
-        <v>1.0500004999999999</v>
-      </c>
-      <c r="F10" s="5">
-        <v>4</v>
-      </c>
-      <c r="G10" s="5">
-        <v>1.0000009999999999</v>
-      </c>
-      <c r="H10" s="5">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M10" s="7"/>
-    </row>
-    <row r="11" spans="1:24" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
-        <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E11" s="5">
         <f>AVERAGE(G11:H11)</f>
-        <v>1.25</v>
+        <v>1.0500004999999999</v>
       </c>
       <c r="F11" s="5">
         <v>4</v>
       </c>
       <c r="G11" s="5">
-        <v>1</v>
+        <v>1.0000009999999999</v>
       </c>
       <c r="H11" s="5">
-        <v>1.5</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
@@ -1306,32 +1401,33 @@
       <c r="L11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="M11" s="5"/>
+      <c r="M11" s="7"/>
     </row>
     <row r="12" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>80</v>
+        <v>125</v>
       </c>
       <c r="E12" s="5">
-        <v>0.05</v>
+        <f>AVERAGE(G12:H12)</f>
+        <v>1.25</v>
       </c>
       <c r="F12" s="5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G12" s="5">
-        <v>0.05</v>
+        <v>1</v>
       </c>
       <c r="H12" s="5">
-        <v>0.1</v>
+        <v>1.5</v>
       </c>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
@@ -1341,30 +1437,30 @@
       </c>
       <c r="M12" s="5"/>
     </row>
-    <row r="13" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E13" s="5">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="F13" s="5">
         <v>5</v>
       </c>
       <c r="G13" s="5">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
       <c r="H13" s="5">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
@@ -1376,28 +1472,28 @@
     </row>
     <row r="14" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E14" s="5">
-        <v>1.2</v>
+        <v>0.1</v>
       </c>
       <c r="F14" s="5">
         <v>5</v>
       </c>
       <c r="G14" s="5">
-        <v>1.01</v>
+        <v>0.01</v>
       </c>
       <c r="H14" s="5">
-        <v>1.7</v>
+        <v>0.2</v>
       </c>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
@@ -1405,32 +1501,32 @@
       <c r="L14" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="M14" s="7"/>
-    </row>
-    <row r="15" spans="1:24" ht="75" x14ac:dyDescent="0.25">
+      <c r="M14" s="5"/>
+    </row>
+    <row r="15" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E15" s="5">
-        <v>0.95</v>
+        <v>1.2</v>
       </c>
       <c r="F15" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G15" s="5">
-        <v>0.5</v>
+        <v>1.01</v>
       </c>
       <c r="H15" s="5">
-        <v>1</v>
+        <v>1.7</v>
       </c>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
@@ -1438,33 +1534,32 @@
       <c r="L15" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="M15" s="5"/>
+      <c r="M15" s="7"/>
     </row>
     <row r="16" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E16" s="5">
-        <f>AVERAGE(G16:H16)</f>
-        <v>-5.5E-2</v>
+        <v>0.95</v>
       </c>
       <c r="F16" s="5">
         <v>4</v>
       </c>
       <c r="G16" s="5">
-        <v>-0.1</v>
+        <v>0.5</v>
       </c>
       <c r="H16" s="5">
-        <v>-0.01</v>
+        <v>1</v>
       </c>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
@@ -1474,162 +1569,163 @@
       </c>
       <c r="M16" s="5"/>
     </row>
-    <row r="17" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
+    <row r="17" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <v>12</v>
+      </c>
       <c r="B17" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E17" s="5">
-        <v>3</v>
+        <f>AVERAGE(G17:H17)</f>
+        <v>-5.5E-2</v>
       </c>
       <c r="F17" s="5">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G17" s="5">
-        <v>3</v>
+        <v>-0.1</v>
       </c>
       <c r="H17" s="5">
-        <v>3</v>
+        <v>-0.01</v>
       </c>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
       <c r="K17" s="5"/>
       <c r="L17" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="M17" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="5">
-        <v>14</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="M17" s="5"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
       <c r="B18" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E18" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F18" s="5">
         <v>6</v>
       </c>
       <c r="G18" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H18" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
       <c r="L18" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="M18" s="5"/>
-    </row>
-    <row r="19" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="M18" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C19" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="D19" s="5" t="s">
-        <v>92</v>
-      </c>
       <c r="E19" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F19" s="5">
         <v>6</v>
       </c>
       <c r="G19" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H19" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
       <c r="L19" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="M19" s="8"/>
-    </row>
-    <row r="20" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="M19" s="5"/>
+    </row>
+    <row r="20" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E20" s="5">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="F20" s="5">
         <v>6</v>
       </c>
       <c r="G20" s="5">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="H20" s="5">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
       <c r="L20" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M20" s="5"/>
-    </row>
-    <row r="21" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="M20" s="8"/>
+    </row>
+    <row r="21" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E21" s="5">
-        <v>1.0009999999999999</v>
+        <v>0.8</v>
       </c>
       <c r="F21" s="5">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G21" s="5">
-        <v>1.0009999999999999</v>
+        <v>0.8</v>
       </c>
       <c r="H21" s="5">
-        <v>1.2</v>
+        <v>0.8</v>
       </c>
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
@@ -1637,20 +1733,20 @@
       <c r="L21" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="M21" s="6"/>
-    </row>
-    <row r="22" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="M21" s="5"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E22" s="5">
         <v>1.0009999999999999</v>
@@ -1670,20 +1766,20 @@
       <c r="L22" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="M22" s="5"/>
-    </row>
-    <row r="23" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="M22" s="6"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E23" s="5">
         <v>1.0009999999999999</v>
@@ -1705,99 +1801,115 @@
       </c>
       <c r="M23" s="5"/>
     </row>
-    <row r="24" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="E24" s="5">
-        <v>4.7999999999999996E-3</v>
+        <v>1.0009999999999999</v>
       </c>
       <c r="F24" s="5">
-        <v>6</v>
-      </c>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
+        <v>4</v>
+      </c>
+      <c r="G24" s="5">
+        <v>1.0009999999999999</v>
+      </c>
+      <c r="H24" s="5">
+        <v>1.2</v>
+      </c>
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
-      <c r="L24" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="M24" s="6" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="L24" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="M24" s="5"/>
+    </row>
+    <row r="25" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>44</v>
+        <v>103</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>46</v>
+        <v>104</v>
       </c>
       <c r="E25" s="5">
-        <v>0.28499999999999998</v>
+        <v>4.7999999999999996E-3</v>
       </c>
       <c r="F25" s="5">
-        <v>5</v>
-      </c>
-      <c r="G25" s="5">
-        <f>E25</f>
-        <v>0.28499999999999998</v>
-      </c>
-      <c r="H25" s="5">
-        <f>(J25-I25)/(2*NORMINV(0.975,0,1))</f>
-        <v>1.6837044078513583E-2</v>
-      </c>
-      <c r="I25" s="5">
-        <v>0.253</v>
-      </c>
-      <c r="J25" s="5">
-        <v>0.31900000000000001</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
       <c r="K25" s="5"/>
       <c r="L25" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="M25" s="6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="5">
+        <v>21</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="M25" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="5"/>
+      <c r="E26" s="5">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="F26" s="5">
+        <v>5</v>
+      </c>
+      <c r="G26" s="5">
+        <f>E26</f>
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="H26" s="5">
+        <f>(J26-I26)/(2*NORMINV(0.975,0,1))</f>
+        <v>1.6837044078513583E-2</v>
+      </c>
+      <c r="I26" s="5">
+        <v>0.253</v>
+      </c>
+      <c r="J26" s="5">
+        <v>0.31900000000000001</v>
+      </c>
       <c r="K26" s="5"/>
-      <c r="L26" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M26" s="5"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L26" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="M26" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
+      <c r="C27" s="6"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
@@ -1806,10 +1918,12 @@
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
-      <c r="L27" s="5"/>
+      <c r="L27" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M27" s="5"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -1824,52 +1938,183 @@
       <c r="L28" s="5"/>
       <c r="M28" s="5"/>
     </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="M33">
-        <v>12</v>
-      </c>
-      <c r="N33">
-        <f>M33*N34/M34</f>
-        <v>0.47213114754098356</v>
-      </c>
-    </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="M34">
-        <v>61</v>
-      </c>
-      <c r="N34">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
+    </row>
+    <row r="30" spans="1:14" s="18" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A30" s="18" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C31" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="E31" s="12">
+        <v>0.23</v>
+      </c>
+      <c r="L31" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="M31" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="N31" s="12" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C32" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="E32" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="L32" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="M32" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="N32" s="12" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="33" spans="2:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C33" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="E33" s="12">
+        <v>0.88</v>
+      </c>
+      <c r="L33" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="M33" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="N33" s="12" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="34" spans="2:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C34" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="E34" s="12">
+        <v>0.95</v>
+      </c>
+      <c r="L34" s="12" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="35" spans="2:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C35" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="E35" s="12">
+        <v>0.54</v>
+      </c>
+      <c r="L35" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="M35" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="N35" s="12">
         <v>2.4</v>
       </c>
     </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
+    <row r="36" spans="2:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C36" s="12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="37" spans="2:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C37" s="12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="38" spans="2:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="C38" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="D38" s="12"/>
+      <c r="E38" s="20">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="F38" s="12">
+        <v>5</v>
+      </c>
+      <c r="G38" s="20">
+        <f>E38</f>
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="H38" s="12">
+        <f>(J38-I38)/(2*NORMINV(0.975,0,1))</f>
+        <v>2.55106728462327E-3</v>
+      </c>
+      <c r="I38" s="20">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="J38" s="20">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="K38" s="12"/>
+      <c r="L38" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="M38" s="12" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>37</v>
+      </c>
+      <c r="C39" t="s">
         <v>38</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D39" t="s">
         <v>39</v>
       </c>
-      <c r="D38" t="s">
+      <c r="E39">
+        <v>4.3200000000000001E-3</v>
+      </c>
+      <c r="G39">
+        <f>E39</f>
+        <v>4.3200000000000001E-3</v>
+      </c>
+      <c r="H39">
+        <f>(J39-I39)/(2*NORMINV(0.975,0,1))</f>
+        <v>1.4285976793890307E-4</v>
+      </c>
+      <c r="I39">
+        <v>4.0400000000000002E-3</v>
+      </c>
+      <c r="J39">
+        <v>4.5999999999999999E-3</v>
+      </c>
+      <c r="L39" t="s">
         <v>40</v>
       </c>
-      <c r="E38">
-        <v>4.3199999999999992E-3</v>
-      </c>
-      <c r="G38">
-        <f>E38</f>
-        <v>4.3199999999999992E-3</v>
-      </c>
-      <c r="H38">
-        <f>(J38-I38)/(2*NORMINV(0.975,0,1))</f>
-        <v>1.4285976793890307E-4</v>
-      </c>
-      <c r="I38">
-        <v>4.0400000000000002E-3</v>
-      </c>
-      <c r="J38">
-        <v>4.5999999999999999E-3</v>
-      </c>
-      <c r="L38" t="s">
-        <v>41</v>
+    </row>
+    <row r="41" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="F41">
+        <f>2.4/5</f>
+        <v>0.48</v>
       </c>
     </row>
   </sheetData>
@@ -1878,8 +2123,8 @@
     <mergeCell ref="I1:J1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="L7" r:id="rId1" xr:uid="{A3AB382F-C46B-41A4-BFA8-DBE37CB64893}"/>
-    <hyperlink ref="L8" r:id="rId2" xr:uid="{E4F5C3E2-0ECA-4597-B6F5-C5FAECC27DA6}"/>
+    <hyperlink ref="L8" r:id="rId1" xr:uid="{A3AB382F-C46B-41A4-BFA8-DBE37CB64893}"/>
+    <hyperlink ref="L9" r:id="rId2" xr:uid="{E4F5C3E2-0ECA-4597-B6F5-C5FAECC27DA6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -1904,7 +2149,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>4</v>
@@ -1913,532 +2158,532 @@
         <v>9</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B2" s="11">
-        <f>parameters!E2</f>
+        <f>parameters!E3</f>
         <v>1E-4</v>
       </c>
       <c r="C2" s="11">
-        <f>parameters!F2</f>
+        <f>parameters!F3</f>
         <v>1</v>
       </c>
       <c r="D2" s="11">
-        <f>parameters!G2</f>
+        <f>parameters!G3</f>
         <v>0.99980000000000002</v>
       </c>
       <c r="E2" s="11">
-        <f>parameters!H2</f>
+        <f>parameters!H3</f>
         <v>9997.0002000000004</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" s="11">
-        <f>parameters!E3</f>
+        <f>parameters!E4</f>
         <v>0.192</v>
       </c>
       <c r="C3" s="11">
-        <f>parameters!F3</f>
+        <f>parameters!F4</f>
         <v>1</v>
       </c>
       <c r="D3" s="11">
-        <f>parameters!G3</f>
+        <f>parameters!G4</f>
         <v>4765.5859199999986</v>
       </c>
       <c r="E3" s="11">
-        <f>parameters!H3</f>
+        <f>parameters!H4</f>
         <v>20055.174079999993</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" s="11">
-        <f>parameters!E4</f>
+        <f>parameters!E5</f>
         <v>1.99</v>
       </c>
       <c r="C4" s="11">
-        <f>parameters!F4</f>
+        <f>parameters!F5</f>
         <v>3</v>
       </c>
       <c r="D4" s="11">
-        <f>parameters!G4</f>
+        <f>parameters!G5</f>
         <v>0.68813463873640102</v>
       </c>
       <c r="E4" s="11">
-        <f>parameters!H4</f>
+        <f>parameters!H5</f>
         <v>0.2507383667215965</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" s="11">
-        <f>parameters!E5</f>
+        <f>parameters!E6</f>
         <v>2.04</v>
       </c>
       <c r="C5" s="11">
-        <f>parameters!F5</f>
+        <f>parameters!F6</f>
         <v>3</v>
       </c>
       <c r="D5" s="11">
-        <f>parameters!G5</f>
+        <f>parameters!G6</f>
         <v>0.71294980785612505</v>
       </c>
       <c r="E5" s="11">
-        <f>parameters!H5</f>
+        <f>parameters!H6</f>
         <v>4.9935758684879816E-2</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6" s="11">
-        <f>parameters!E6</f>
+        <f>parameters!E7</f>
         <v>3.47</v>
       </c>
       <c r="C6" s="11">
-        <f>parameters!F6</f>
+        <f>parameters!F7</f>
         <v>3</v>
       </c>
       <c r="D6" s="11">
-        <f>parameters!G6</f>
+        <f>parameters!G7</f>
         <v>1.2441545939587679</v>
       </c>
       <c r="E6" s="11">
-        <f>parameters!H6</f>
+        <f>parameters!H7</f>
         <v>6.1700065487409E-2</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="str">
-        <f>parameters!D7</f>
+        <f>parameters!D8</f>
         <v>RR.All.Death.past_smoke</v>
       </c>
       <c r="B7" s="11">
-        <f>parameters!E7</f>
+        <f>parameters!E8</f>
         <v>1.2</v>
       </c>
       <c r="C7" s="11">
-        <f>parameters!F7</f>
+        <f>parameters!F8</f>
         <v>3</v>
       </c>
       <c r="D7" s="11">
-        <f>parameters!G7</f>
+        <f>parameters!G8</f>
         <v>0.18232155679395459</v>
       </c>
       <c r="E7" s="11">
-        <f>parameters!H7</f>
+        <f>parameters!H8</f>
         <v>2.5531963685666733E-2</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="str">
-        <f>parameters!D8</f>
+        <f>parameters!D9</f>
         <v>RR.All.Death.current_smoke</v>
       </c>
       <c r="B8" s="11">
-        <f>parameters!E8</f>
+        <f>parameters!E9</f>
         <v>2.76</v>
       </c>
       <c r="C8" s="11">
-        <f>parameters!F8</f>
+        <f>parameters!F9</f>
         <v>3</v>
       </c>
       <c r="D8" s="11">
-        <f>parameters!G8</f>
+        <f>parameters!G9</f>
         <v>1.0152306797290584</v>
       </c>
       <c r="E8" s="11">
-        <f>parameters!H8</f>
+        <f>parameters!H9</f>
         <v>9.2440087521680724E-3</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="str">
-        <f>parameters!D9</f>
+        <f>parameters!D10</f>
         <v>P.quit.smoke</v>
       </c>
       <c r="B9" s="11">
-        <f>parameters!E9</f>
+        <f>parameters!E10</f>
         <v>1.67E-2</v>
       </c>
       <c r="C9" s="11">
-        <f>parameters!F9</f>
+        <f>parameters!F10</f>
         <v>5</v>
       </c>
       <c r="D9" s="11">
-        <f>parameters!G9</f>
+        <f>parameters!G10</f>
         <v>1.67E-2</v>
       </c>
       <c r="E9" s="11">
-        <f>parameters!H9</f>
+        <f>parameters!H10</f>
         <v>4.0523713428230627E-4</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="str">
-        <f>parameters!D10</f>
+        <f>parameters!D11</f>
         <v>P.onset_age</v>
       </c>
       <c r="B10" s="11">
-        <f>parameters!E10</f>
+        <f>parameters!E11</f>
         <v>1.0500004999999999</v>
       </c>
       <c r="C10" s="11">
-        <f>parameters!F10</f>
+        <f>parameters!F11</f>
         <v>4</v>
       </c>
       <c r="D10" s="11">
-        <f>parameters!G10</f>
+        <f>parameters!G11</f>
         <v>1.0000009999999999</v>
       </c>
       <c r="E10" s="11">
-        <f>parameters!H10</f>
+        <f>parameters!H11</f>
         <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="str">
-        <f>parameters!D11</f>
-        <v>P.onset_sex</v>
+        <f>parameters!D12</f>
+        <v>RR.onset_sex</v>
       </c>
       <c r="B11" s="11">
-        <f>parameters!E11</f>
+        <f>parameters!E12</f>
         <v>1.25</v>
       </c>
       <c r="C11" s="11">
-        <f>parameters!F11</f>
+        <f>parameters!F12</f>
         <v>4</v>
       </c>
       <c r="D11" s="11">
-        <f>parameters!G11</f>
+        <f>parameters!G12</f>
         <v>1</v>
       </c>
       <c r="E11" s="11">
-        <f>parameters!H11</f>
+        <f>parameters!H12</f>
         <v>1.5</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="str">
-        <f>parameters!D12</f>
+        <f>parameters!D13</f>
         <v>P.sympt.diag_LGBC</v>
       </c>
       <c r="B12" s="11">
-        <f>parameters!E12</f>
+        <f>parameters!E13</f>
         <v>0.05</v>
       </c>
       <c r="C12" s="11">
-        <f>parameters!F12</f>
+        <f>parameters!F13</f>
         <v>5</v>
       </c>
       <c r="D12" s="11">
-        <f>parameters!G12</f>
+        <f>parameters!G13</f>
         <v>0.05</v>
       </c>
       <c r="E12" s="11">
-        <f>parameters!H12</f>
+        <f>parameters!H13</f>
         <v>0.1</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="str">
-        <f>parameters!D13</f>
+        <f>parameters!D14</f>
         <v>P.sympt.diag_A_HGBC</v>
       </c>
       <c r="B13" s="11">
-        <f>parameters!E13</f>
+        <f>parameters!E14</f>
         <v>0.1</v>
       </c>
       <c r="C13" s="11">
-        <f>parameters!F13</f>
+        <f>parameters!F14</f>
         <v>5</v>
       </c>
       <c r="D13" s="11">
-        <f>parameters!G13</f>
+        <f>parameters!G14</f>
         <v>0.01</v>
       </c>
       <c r="E13" s="11">
-        <f>parameters!H13</f>
+        <f>parameters!H14</f>
         <v>0.2</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="str">
-        <f>parameters!D14</f>
+        <f>parameters!D15</f>
         <v>P.sympt.diag_B_HGBC</v>
       </c>
       <c r="B14" s="11">
-        <f>parameters!E14</f>
+        <f>parameters!E15</f>
         <v>1.2</v>
       </c>
       <c r="C14" s="11">
-        <f>parameters!F14</f>
+        <f>parameters!F15</f>
         <v>5</v>
       </c>
       <c r="D14" s="11">
-        <f>parameters!G14</f>
+        <f>parameters!G15</f>
         <v>1.01</v>
       </c>
       <c r="E14" s="11">
-        <f>parameters!H14</f>
+        <f>parameters!H15</f>
         <v>1.7</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="str">
-        <f>parameters!D15</f>
+        <f>parameters!D16</f>
         <v>P.sympt.diag_Age80_HGBC</v>
       </c>
       <c r="B15" s="11">
-        <f>parameters!E15</f>
+        <f>parameters!E16</f>
         <v>0.95</v>
       </c>
       <c r="C15" s="11">
-        <f>parameters!F15</f>
+        <f>parameters!F16</f>
         <v>4</v>
       </c>
       <c r="D15" s="11">
-        <f>parameters!G15</f>
+        <f>parameters!G16</f>
         <v>0.5</v>
       </c>
       <c r="E15" s="11">
-        <f>parameters!H15</f>
+        <f>parameters!H16</f>
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="str">
-        <f>parameters!D16</f>
+        <f>parameters!D17</f>
         <v>C.age.80.undiag.mort</v>
       </c>
       <c r="B16" s="11">
-        <f>parameters!E16</f>
+        <f>parameters!E17</f>
         <v>-5.5E-2</v>
       </c>
       <c r="C16" s="11">
-        <f>parameters!F16</f>
+        <f>parameters!F17</f>
         <v>4</v>
       </c>
       <c r="D16" s="11">
-        <f>parameters!G16</f>
+        <f>parameters!G17</f>
         <v>-0.1</v>
       </c>
       <c r="E16" s="11">
-        <f>parameters!H16</f>
+        <f>parameters!H17</f>
         <v>-0.01</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="str">
-        <f>parameters!D17</f>
+        <f>parameters!D18</f>
         <v>Mean.t.StI.StII</v>
       </c>
       <c r="B17" s="11">
-        <f>parameters!E17</f>
+        <f>parameters!E18</f>
         <v>3</v>
       </c>
       <c r="C17" s="11">
-        <f>parameters!F17</f>
+        <f>parameters!F18</f>
         <v>6</v>
       </c>
       <c r="D17" s="11">
-        <f>parameters!G17</f>
+        <f>parameters!G18</f>
         <v>3</v>
       </c>
       <c r="E17" s="11">
-        <f>parameters!H17</f>
+        <f>parameters!H18</f>
         <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
-        <f>parameters!D18</f>
+        <f>parameters!D19</f>
         <v>Mean.t.StII.StIII</v>
       </c>
       <c r="B18">
-        <f>parameters!E18</f>
+        <f>parameters!E19</f>
         <v>2</v>
       </c>
       <c r="C18">
-        <f>parameters!F18</f>
+        <f>parameters!F19</f>
         <v>6</v>
       </c>
       <c r="D18">
-        <f>parameters!G18</f>
+        <f>parameters!G19</f>
         <v>2</v>
       </c>
       <c r="E18">
-        <f>parameters!H18</f>
+        <f>parameters!H19</f>
         <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
-        <f>parameters!D19</f>
+        <f>parameters!D20</f>
         <v>Mean.t.StIII.StIV</v>
       </c>
       <c r="B19">
-        <f>parameters!E19</f>
+        <f>parameters!E20</f>
         <v>1</v>
       </c>
       <c r="C19">
-        <f>parameters!F19</f>
+        <f>parameters!F20</f>
         <v>6</v>
       </c>
       <c r="D19">
-        <f>parameters!G19</f>
+        <f>parameters!G20</f>
         <v>1</v>
       </c>
       <c r="E19">
-        <f>parameters!H19</f>
+        <f>parameters!H20</f>
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
-        <f>parameters!D20</f>
+        <f>parameters!D21</f>
         <v>RR.All.Death.no_smoke</v>
       </c>
       <c r="B20">
-        <f>parameters!E20</f>
+        <f>parameters!E21</f>
         <v>0.8</v>
       </c>
       <c r="C20">
-        <f>parameters!F20</f>
+        <f>parameters!F21</f>
         <v>6</v>
       </c>
       <c r="D20">
-        <f>parameters!G20</f>
+        <f>parameters!G21</f>
         <v>0.8</v>
       </c>
       <c r="E20">
-        <f>parameters!H20</f>
+        <f>parameters!H21</f>
         <v>0.8</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
-        <f>parameters!D21</f>
+        <f>parameters!D22</f>
         <v>shape.t.StI.StII</v>
       </c>
       <c r="B21">
-        <f>parameters!E21</f>
+        <f>parameters!E22</f>
         <v>1.0009999999999999</v>
       </c>
       <c r="C21">
-        <f>parameters!F21</f>
+        <f>parameters!F22</f>
         <v>4</v>
       </c>
       <c r="D21">
-        <f>parameters!G21</f>
+        <f>parameters!G22</f>
         <v>1.0009999999999999</v>
       </c>
       <c r="E21">
-        <f>parameters!H21</f>
+        <f>parameters!H22</f>
         <v>1.2</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
-        <f>parameters!D22</f>
+        <f>parameters!D23</f>
         <v>shape.t.StII.StIII</v>
       </c>
       <c r="B22">
-        <f>parameters!E22</f>
+        <f>parameters!E23</f>
         <v>1.0009999999999999</v>
       </c>
       <c r="C22">
-        <f>parameters!F22</f>
+        <f>parameters!F23</f>
         <v>4</v>
       </c>
       <c r="D22">
-        <f>parameters!G22</f>
+        <f>parameters!G23</f>
         <v>1.0009999999999999</v>
       </c>
       <c r="E22">
-        <f>parameters!H22</f>
+        <f>parameters!H23</f>
         <v>1.2</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
-        <f>parameters!D23</f>
+        <f>parameters!D24</f>
         <v>shape.t.StIII.StIV</v>
       </c>
       <c r="B23">
-        <f>parameters!E23</f>
+        <f>parameters!E24</f>
         <v>1.0009999999999999</v>
       </c>
       <c r="C23">
-        <f>parameters!F23</f>
+        <f>parameters!F24</f>
         <v>4</v>
       </c>
       <c r="D23">
-        <f>parameters!G23</f>
+        <f>parameters!G24</f>
         <v>1.0009999999999999</v>
       </c>
       <c r="E23">
-        <f>parameters!H23</f>
+        <f>parameters!H24</f>
         <v>1.2</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
-        <f>parameters!D24</f>
+        <f>parameters!D25</f>
         <v>P.LGtoHGBC</v>
       </c>
       <c r="B24">
-        <f>parameters!E24</f>
+        <f>parameters!E25</f>
         <v>4.7999999999999996E-3</v>
       </c>
       <c r="C24">
-        <f>parameters!F24</f>
+        <f>parameters!F25</f>
         <v>6</v>
       </c>
       <c r="D24">
-        <f>parameters!G24</f>
+        <f>parameters!G25</f>
         <v>0</v>
       </c>
       <c r="E24">
-        <f>parameters!H24</f>
+        <f>parameters!H25</f>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
-        <f>parameters!D25</f>
+        <f>parameters!D26</f>
         <v>P.Recurrence.LR</v>
       </c>
       <c r="B25">
-        <f>parameters!E25</f>
+        <f>parameters!E26</f>
         <v>0.28499999999999998</v>
       </c>
       <c r="C25">
-        <f>parameters!F25</f>
+        <f>parameters!F26</f>
         <v>5</v>
       </c>
       <c r="D25">
-        <f>parameters!G25</f>
+        <f>parameters!G26</f>
         <v>0.28499999999999998</v>
       </c>
       <c r="E25">
-        <f>parameters!H25</f>
+        <f>parameters!H26</f>
         <v>1.6837044078513583E-2</v>
       </c>
     </row>
@@ -2522,10 +2767,10 @@
     </row>
     <row r="6" spans="2:26" x14ac:dyDescent="0.25">
       <c r="L6" t="s">
+        <v>76</v>
+      </c>
+      <c r="M6" t="s">
         <v>77</v>
-      </c>
-      <c r="M6" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="7" spans="2:26" x14ac:dyDescent="0.25">
@@ -2542,7 +2787,7 @@
         <v>25</v>
       </c>
       <c r="K7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L7">
         <v>1.01</v>
@@ -2588,7 +2833,7 @@
         <v>0.10100000000000001</v>
       </c>
       <c r="P9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="2:26" x14ac:dyDescent="0.25">
@@ -3127,6 +3372,29 @@
     <row r="33" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C33">
         <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06CC0F33-7270-4213-838D-9B3F1B62F32F}">
+  <dimension ref="E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="26.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>